<commit_message>
note re: supporting EDTF
</commit_message>
<xml_diff>
--- a/notes/tsv-columns_new.xlsx
+++ b/notes/tsv-columns_new.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -80,30 +80,15 @@
     <t>ccodes</t>
   </si>
   <si>
-    <t>One or more modern 2-letter country codes (used purely for locative purposes; does not indicate a relationship)</t>
-  </si>
-  <si>
     <t>types</t>
   </si>
   <si>
-    <t>One or more pipe (|) delimited name and language variants; can be suffixed with @ + language-script code if available</t>
-  </si>
-  <si>
-    <t>One or more pipe (|) delimited terms for place type (contributor's term, e.g. pueblo)</t>
-  </si>
-  <si>
     <t>aat_typeid</t>
   </si>
   <si>
     <t>matches</t>
   </si>
   <si>
-    <t>One or more pipe (|) delimited URIs for matching record(s) in place name authority resources; includes 'exact' and 'close' matches</t>
-  </si>
-  <si>
-    <t>One or more pipe (|) delimited AAT integer identifiers from WHG's subset list of 160 place type concepts</t>
-  </si>
-  <si>
     <t>parent_name</t>
   </si>
   <si>
@@ -131,19 +116,37 @@
     <t>Latitude for point geometry; decimal degrees</t>
   </si>
   <si>
-    <t>geom_srclabel</t>
-  </si>
-  <si>
-    <t>geom_srcid</t>
-  </si>
-  <si>
-    <t>Label or short citation for source of the geometry</t>
-  </si>
-  <si>
-    <t>URI identifier for the source of the geometry</t>
-  </si>
-  <si>
-    <t>Any geometry in WKT format; polygons should be simplified, using GIS function or https://mapshaper.org/; will supercede lon/lat, if given</t>
+    <t>opt</t>
+  </si>
+  <si>
+    <t>URI identifier for the source of the geometry, e.g.  http://www.geonames.org/2950159</t>
+  </si>
+  <si>
+    <t>Label or short citation for source of the geometry, e.g. GeoNames</t>
+  </si>
+  <si>
+    <t>geo_srclabel</t>
+  </si>
+  <si>
+    <t>geo_srcid</t>
+  </si>
+  <si>
+    <t>Any geometry in WKT format; polygons should be simplified for rendering performance, using e.g. a GIS function or https://mapshaper.org/; will supercede lon/lat, if both are supplied</t>
+  </si>
+  <si>
+    <t>One or more name and language variants; can be suffixed with @ + language-script code if available</t>
+  </si>
+  <si>
+    <t>One or more URIs for matching record(s) in place name authority resources; includes 'exact' and 'close' matches</t>
+  </si>
+  <si>
+    <t>One or more terms for place type (contributor's term, e.g. pueblo)</t>
+  </si>
+  <si>
+    <t>One or more AAT integer identifiers from WHG's subset list of 160 place type concepts</t>
+  </si>
+  <si>
+    <t>One or more ISO Alpha-2 two-letter country codes (used purely for locative purposes; does not indicate a relationship)</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,99 +545,135 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
         <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>